<commit_message>
Commit before starting new track changes
Lots of update: Would remove unrelavant files in the subsequent commit
</commit_message>
<xml_diff>
--- a/Programs/Extracted Data/AlphaFeedback_Subject_analysis.xlsx
+++ b/Programs/Extracted Data/AlphaFeedback_Subject_analysis.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Projects\AlphaFeedbackProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RayLabCNS\Documents\MATLAB\Ankan_M\AlphaFeedbackProject_Ver_Latest_Local\Programs\Extracted Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F8A4FB-9BC6-4E81-AAE2-6608A7C3781B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="8115" xr2:uid="{70965B6E-8483-4C99-9D6B-FEB0B4BB4BDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Subject No</t>
   </si>
@@ -225,12 +226,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -550,14 +551,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2155804-4DCB-4489-A947-ADDD539C2A27}">
-  <dimension ref="B2:M28"/>
+  <dimension ref="A2:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
@@ -568,63 +570,69 @@
     <col min="13" max="13" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="4" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4" t="s">
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4" t="s">
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="8" t="s">
+      <c r="L2" s="8"/>
+      <c r="M2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="7" t="s">
         <v>30</v>
       </c>
       <c r="M3" s="3"/>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
       <c r="B5">
         <v>1</v>
       </c>
@@ -658,7 +666,11 @@
         <v>0.35439999999999999</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>A5+1</f>
+        <v>2</v>
+      </c>
       <c r="B6">
         <f>B5+1</f>
         <v>2</v>
@@ -693,9 +705,13 @@
         <v>0.14329999999999998</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" ref="A7:A14" si="2">A6+1</f>
+        <v>3</v>
+      </c>
       <c r="B7">
-        <f t="shared" ref="B7:B27" si="2">B6+1</f>
+        <f t="shared" ref="B7:B27" si="3">B6+1</f>
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -728,11 +744,15 @@
         <v>8.0999999999999961E-3</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
+      <c r="B8">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
@@ -763,11 +783,15 @@
         <v>0.16790000000000005</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
+      <c r="B9">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>6</v>
       </c>
@@ -798,11 +822,15 @@
         <v>1.3199999999999878E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
+      <c r="B10">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
@@ -833,11 +861,15 @@
         <v>-5.710000000000004E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
+      <c r="B11">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
@@ -868,9 +900,13 @@
         <v>0.29720000000000002</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
       <c r="B12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -903,31 +939,35 @@
         <v>-1.9000000000000128E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="5">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5" t="s">
+      <c r="B13" s="4">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>10</v>
       </c>
-      <c r="F13" s="5">
-        <v>1</v>
-      </c>
-      <c r="G13" s="5">
-        <v>1</v>
-      </c>
-      <c r="H13" s="5">
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1</v>
+      </c>
+      <c r="H13" s="4">
         <v>1.3310999999999999</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="4">
         <v>1.3393999999999999</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="4">
         <v>1.3935999999999999</v>
       </c>
       <c r="K13">
@@ -939,12 +979,16 @@
         <v>-6.25E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="B14">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E14">
@@ -974,12 +1018,15 @@
         <v>4.9200000000000021E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>201</v>
+      </c>
       <c r="B15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E15">
@@ -1009,9 +1056,13 @@
         <v>-7.3000000000000842E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f>A15+1</f>
+        <v>202</v>
+      </c>
       <c r="B16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="D16" t="s">
@@ -1044,15 +1095,19 @@
         <v>6.2999999999999723E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" ref="A17:A28" si="4">A16+1</f>
+        <v>203</v>
+      </c>
       <c r="B17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="D17" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>8</v>
       </c>
       <c r="F17">
@@ -1079,9 +1134,13 @@
         <v>-1.0599999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="4"/>
+        <v>204</v>
+      </c>
       <c r="B18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="D18" t="s">
@@ -1114,9 +1173,13 @@
         <v>0.11670000000000003</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="4"/>
+        <v>205</v>
+      </c>
       <c r="B19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="D19" t="s">
@@ -1149,9 +1212,13 @@
         <v>1.6699999999999993E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="4"/>
+        <v>206</v>
+      </c>
       <c r="B20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="D20" t="s">
@@ -1184,9 +1251,13 @@
         <v>0.15110000000000001</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="4"/>
+        <v>207</v>
+      </c>
       <c r="B21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="D21" t="s">
@@ -1219,9 +1290,13 @@
         <v>-2.52E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="4"/>
+        <v>208</v>
+      </c>
       <c r="B22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="D22" t="s">
@@ -1254,9 +1329,13 @@
         <v>-2.189999999999992E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="4"/>
+        <v>209</v>
+      </c>
       <c r="B23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="D23" t="s">
@@ -1289,9 +1368,13 @@
         <v>1.0999999999999899E-3</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="4"/>
+        <v>210</v>
+      </c>
       <c r="B24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="D24" t="s">
@@ -1324,15 +1407,19 @@
         <v>1.7900000000000027E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="4"/>
+        <v>211</v>
+      </c>
       <c r="B25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="D25" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="4">
         <v>9</v>
       </c>
       <c r="F25">
@@ -1359,9 +1446,13 @@
         <v>0.10830000000000006</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="4"/>
+        <v>212</v>
+      </c>
       <c r="B26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="D26" t="s">
@@ -1394,9 +1485,13 @@
         <v>2.5299999999999989E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="4"/>
+        <v>213</v>
+      </c>
       <c r="B27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="D27" t="s">
@@ -1429,7 +1524,11 @@
         <v>7.580000000000009E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="4"/>
+        <v>214</v>
+      </c>
       <c r="B28">
         <f>B27+1</f>
         <v>24</v>

</xml_diff>